<commit_message>
Bulk CIs data updated
</commit_message>
<xml_diff>
--- a/src/test/resources/Test Attachments/50 CI's/50CIsXLSX.xlsx
+++ b/src/test/resources/Test Attachments/50 CI's/50CIsXLSX.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlm97\Documents\oneworkflow-automation\src\test\resources\Test Attachments\50 CI's\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drmay\Downloads\Test Attachments\50 CI's\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F17D52-60F7-44D6-AF6D-F3AFFBB946B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1951ECA-5D69-4CB7-8027-66617A569201}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="588" windowWidth="17280" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="792" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CIList" sheetId="1" r:id="rId1"/>
@@ -169,20 +169,20 @@
     <t>DK_AAA_AAA01DK</t>
   </si>
   <si>
-    <t>dk gdpr purpose</t>
-  </si>
-  <si>
-    <t>DK_AAA_AAA02DK</t>
-  </si>
-  <si>
-    <t>SE_AAA_TestMartinx</t>
+    <t>selanne</t>
+  </si>
+  <si>
+    <t>SELYCAL01S-FLX</t>
+  </si>
+  <si>
+    <t>Selleri ACC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -190,16 +190,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD2D3D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -207,15 +219,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFEEEEEE"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,271 +553,946 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A51"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:W51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49:B50"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="T28">
+        <v>1</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="T30">
+        <v>1</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="T31">
+        <v>1</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="T32">
+        <v>1</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="T33">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="T34">
+        <v>1</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="T35">
+        <v>1</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="T36">
+        <v>1</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="T37">
+        <v>1</v>
+      </c>
+      <c r="U37">
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="T38">
+        <v>1</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="T39">
+        <v>1</v>
+      </c>
+      <c r="U39">
+        <v>0</v>
+      </c>
+      <c r="V39">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="T40">
+        <v>1</v>
+      </c>
+      <c r="U40">
+        <v>0</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="U41">
+        <v>0</v>
+      </c>
+      <c r="V41">
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="T42">
+        <v>1</v>
+      </c>
+      <c r="U42">
+        <v>0</v>
+      </c>
+      <c r="V42">
+        <v>0</v>
+      </c>
+      <c r="W42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="T43">
+        <v>1</v>
+      </c>
+      <c r="U43">
+        <v>0</v>
+      </c>
+      <c r="V43">
+        <v>0</v>
+      </c>
+      <c r="W43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="T44">
+        <v>1</v>
+      </c>
+      <c r="U44">
+        <v>0</v>
+      </c>
+      <c r="V44">
+        <v>0</v>
+      </c>
+      <c r="W44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="T45">
+        <v>1</v>
+      </c>
+      <c r="U45">
+        <v>0</v>
+      </c>
+      <c r="V45">
+        <v>0</v>
+      </c>
+      <c r="W45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="T46">
+        <v>1</v>
+      </c>
+      <c r="U46">
+        <v>0</v>
+      </c>
+      <c r="V46">
+        <v>0</v>
+      </c>
+      <c r="W46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="T47">
+        <v>1</v>
+      </c>
+      <c r="U47">
+        <v>0</v>
+      </c>
+      <c r="V47">
+        <v>0</v>
+      </c>
+      <c r="W47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="T48">
+        <v>1</v>
+      </c>
+      <c r="U48">
+        <v>0</v>
+      </c>
+      <c r="V48">
+        <v>0</v>
+      </c>
+      <c r="W48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="T49">
+        <v>1</v>
+      </c>
+      <c r="U49">
+        <v>0</v>
+      </c>
+      <c r="V49">
+        <v>0</v>
+      </c>
+      <c r="W49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>